<commit_message>
cloning ok-Manar  data needs cleaning
</commit_message>
<xml_diff>
--- a/client/db_titres.xlsx
+++ b/client/db_titres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylila\Desktop\PriceSomeShit\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ylila\Desktop\Pricer 2.0\client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08B6089-1F31-44FE-9694-BEA40ABC830D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B92B09-1990-4C16-A3F4-423AEC964D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1095" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="db_titres" sheetId="1" r:id="rId1"/>
@@ -3095,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A1365" workbookViewId="0">
+      <selection activeCell="D1399" sqref="D1399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84150,14 +84150,6 @@
       <c r="I1369" s="1"/>
       <c r="K1369" s="2"/>
       <c r="L1369" s="2"/>
-      <c r="U1369" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1369">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1370" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1370" s="1"/>
@@ -84167,14 +84159,6 @@
       <c r="I1370" s="1"/>
       <c r="K1370" s="2"/>
       <c r="L1370" s="2"/>
-      <c r="U1370" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1370">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1371" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1371" s="1"/>
@@ -84184,14 +84168,6 @@
       <c r="I1371" s="1"/>
       <c r="K1371" s="2"/>
       <c r="L1371" s="2"/>
-      <c r="U1371" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1371">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1372" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1372" s="1"/>
@@ -84202,14 +84178,6 @@
       <c r="I1372" s="1"/>
       <c r="K1372" s="2"/>
       <c r="L1372" s="2"/>
-      <c r="U1372" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1372">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1373" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1373" s="1"/>
@@ -84220,14 +84188,6 @@
       <c r="J1373" s="1"/>
       <c r="K1373" s="2"/>
       <c r="L1373" s="2"/>
-      <c r="U1373" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1373">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1374" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1374" s="1"/>
@@ -84238,14 +84198,6 @@
       <c r="J1374" s="1"/>
       <c r="K1374" s="2"/>
       <c r="L1374" s="2"/>
-      <c r="U1374" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1374">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1375" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1375" s="1"/>
@@ -84255,14 +84207,6 @@
       <c r="I1375" s="1"/>
       <c r="K1375" s="2"/>
       <c r="L1375" s="2"/>
-      <c r="U1375" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1375">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1376" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1376" s="1"/>
@@ -84272,16 +84216,8 @@
       <c r="I1376" s="1"/>
       <c r="K1376" s="2"/>
       <c r="L1376" s="2"/>
-      <c r="U1376" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1376">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1377" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1377" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1377" s="1"/>
       <c r="C1377"/>
       <c r="G1377" s="3"/>
@@ -84289,16 +84225,8 @@
       <c r="I1377" s="1"/>
       <c r="K1377" s="2"/>
       <c r="L1377" s="2"/>
-      <c r="U1377" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1377">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1378" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1378" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1378" s="1"/>
       <c r="C1378"/>
       <c r="G1378" s="3"/>
@@ -84306,16 +84234,8 @@
       <c r="I1378" s="1"/>
       <c r="K1378" s="2"/>
       <c r="L1378" s="2"/>
-      <c r="U1378" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1378">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1379" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1379" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1379" s="1"/>
       <c r="C1379"/>
       <c r="F1379" s="2"/>
@@ -84324,16 +84244,8 @@
       <c r="I1379" s="1"/>
       <c r="K1379" s="2"/>
       <c r="L1379" s="2"/>
-      <c r="U1379" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1379">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1380" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1380" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1380" s="1"/>
       <c r="C1380"/>
       <c r="F1380" s="2"/>
@@ -84342,16 +84254,8 @@
       <c r="I1380" s="1"/>
       <c r="K1380" s="2"/>
       <c r="L1380" s="2"/>
-      <c r="U1380" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1380">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1381" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1381" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1381" s="1"/>
       <c r="C1381"/>
       <c r="G1381" s="3"/>
@@ -84359,16 +84263,8 @@
       <c r="I1381" s="1"/>
       <c r="K1381" s="2"/>
       <c r="L1381" s="2"/>
-      <c r="U1381" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1381">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1382" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1382" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1382" s="1"/>
       <c r="C1382"/>
       <c r="G1382" s="3"/>
@@ -84376,16 +84272,8 @@
       <c r="I1382" s="1"/>
       <c r="K1382" s="2"/>
       <c r="L1382" s="2"/>
-      <c r="U1382" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1382">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1383" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1383" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1383" s="1"/>
       <c r="C1383"/>
       <c r="G1383" s="3"/>
@@ -84393,16 +84281,8 @@
       <c r="I1383" s="1"/>
       <c r="K1383" s="2"/>
       <c r="L1383" s="2"/>
-      <c r="U1383" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1383">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1384" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1384" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1384" s="1"/>
       <c r="C1384"/>
       <c r="G1384" s="3"/>
@@ -84410,16 +84290,8 @@
       <c r="I1384" s="1"/>
       <c r="K1384" s="2"/>
       <c r="L1384" s="2"/>
-      <c r="U1384" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1384">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1385" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1385" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1385" s="1"/>
       <c r="C1385"/>
       <c r="F1385" s="2"/>
@@ -84428,16 +84300,8 @@
       <c r="I1385" s="1"/>
       <c r="K1385" s="2"/>
       <c r="L1385" s="2"/>
-      <c r="U1385" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1385">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1386" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1386" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1386" s="1"/>
       <c r="C1386"/>
       <c r="G1386" s="3"/>
@@ -84445,16 +84309,8 @@
       <c r="I1386" s="1"/>
       <c r="K1386" s="2"/>
       <c r="L1386" s="2"/>
-      <c r="U1386" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1386">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1387" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1387" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1387" s="1"/>
       <c r="C1387"/>
       <c r="G1387" s="3"/>
@@ -84462,16 +84318,8 @@
       <c r="I1387" s="1"/>
       <c r="K1387" s="2"/>
       <c r="L1387" s="2"/>
-      <c r="U1387" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1387">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1388" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1388" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1388" s="1"/>
       <c r="C1388"/>
       <c r="G1388" s="3"/>
@@ -84479,16 +84327,8 @@
       <c r="I1388" s="1"/>
       <c r="K1388" s="2"/>
       <c r="L1388" s="2"/>
-      <c r="U1388" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1388">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1389" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1389" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1389" s="1"/>
       <c r="C1389"/>
       <c r="G1389" s="3"/>
@@ -84496,16 +84336,8 @@
       <c r="I1389" s="1"/>
       <c r="K1389" s="2"/>
       <c r="L1389" s="2"/>
-      <c r="U1389" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1389">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1390" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1390" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1390" s="1"/>
       <c r="C1390"/>
       <c r="G1390" s="3"/>
@@ -84513,16 +84345,8 @@
       <c r="I1390" s="1"/>
       <c r="K1390" s="2"/>
       <c r="L1390" s="2"/>
-      <c r="U1390" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1390">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1391" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1391" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1391" s="1"/>
       <c r="C1391"/>
       <c r="G1391" s="3"/>
@@ -84530,16 +84354,8 @@
       <c r="I1391" s="1"/>
       <c r="K1391" s="2"/>
       <c r="L1391" s="2"/>
-      <c r="U1391" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1391">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1392" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1392" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1392" s="1"/>
       <c r="C1392"/>
       <c r="G1392" s="3"/>
@@ -84547,14 +84363,6 @@
       <c r="I1392" s="1"/>
       <c r="K1392" s="2"/>
       <c r="L1392" s="2"/>
-      <c r="U1392" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1392">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1393" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1393" s="1"/>
@@ -84564,14 +84372,6 @@
       <c r="I1393" s="1"/>
       <c r="K1393" s="2"/>
       <c r="L1393" s="2"/>
-      <c r="U1393" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1393">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1394" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1394" s="1"/>
@@ -84582,14 +84382,6 @@
       <c r="I1394" s="1"/>
       <c r="K1394" s="2"/>
       <c r="L1394" s="2"/>
-      <c r="U1394" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1394">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1395" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1395" s="1"/>
@@ -84599,14 +84391,6 @@
       <c r="I1395" s="1"/>
       <c r="K1395" s="2"/>
       <c r="L1395" s="2"/>
-      <c r="U1395" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1395">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1396" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1396" s="1"/>
@@ -84616,14 +84400,6 @@
       <c r="I1396" s="1"/>
       <c r="K1396" s="2"/>
       <c r="L1396" s="2"/>
-      <c r="U1396" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1396">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1397" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1397" s="1"/>
@@ -84633,14 +84409,6 @@
       <c r="I1397" s="1"/>
       <c r="K1397" s="2"/>
       <c r="L1397" s="2"/>
-      <c r="U1397" t="str">
-        <f>IFERROR(INDEX([1]!Tableau7[[#All],[DESCRIPTION]],MATCH(Tableau1[[#This Row],[EMETTEUR]],[1]!Tableau7[[#All],[CODE]],0)),"")</f>
-        <v/>
-      </c>
-      <c r="V1397">
-        <f>Tableau1[[#This Row],[TOTAL_VALO]]*Tableau1[[#This Row],[SENSIBILITE]]</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="1399" spans="1:22" x14ac:dyDescent="0.25">
       <c r="V1399" s="3"/>

</xml_diff>